<commit_message>
AMM updated transcript_eval_count documentation
</commit_message>
<xml_diff>
--- a/nanni_maize_2021/documentation/transcriptome_evaluation_counting.xlsx
+++ b/nanni_maize_2021/documentation/transcriptome_evaluation_counting.xlsx
@@ -1487,7 +1487,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1525,10 +1525,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1558,18 +1554,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1665,20 +1649,20 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C94" activeCellId="0" sqref="C94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="37.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="61.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="61.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.66"/>
   </cols>
   <sheetData>
@@ -1872,77 +1856,77 @@
       </c>
     </row>
     <row r="16" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" s="9" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+    <row r="17" s="7" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" s="9" customFormat="true" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
+    <row r="19" s="7" customFormat="true" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" s="9" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" s="9" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+    <row r="20" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" s="7" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1977,37 +1961,37 @@
       <c r="A29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2040,29 +2024,29 @@
     <row r="34" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" s="11" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="s">
+    <row r="37" s="10" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H37" s="10" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2120,7 +2104,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" s="12" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="43" s="4" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>23</v>
@@ -2189,43 +2173,43 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" s="12" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" s="13" customFormat="true" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="13" t="s">
+    <row r="48" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" s="12" customFormat="true" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D49" s="13" t="s">
         <v>109</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-    </row>
-    <row r="51" s="17" customFormat="true" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+    </row>
+    <row r="51" s="16" customFormat="true" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="13" t="s">
         <v>115</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -2240,70 +2224,70 @@
       <c r="H51" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="I51" s="16"/>
-      <c r="J51" s="16"/>
-    </row>
-    <row r="52" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+    </row>
+    <row r="52" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="16"/>
-      <c r="J52" s="16"/>
-    </row>
-    <row r="53" s="10" customFormat="true" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="10" t="s">
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+    </row>
+    <row r="53" s="9" customFormat="true" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>120</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="9" t="s">
         <v>122</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="G53" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="H53" s="10" t="s">
+      <c r="H53" s="9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="54" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="16"/>
-      <c r="J54" s="16"/>
-    </row>
-    <row r="55" s="17" customFormat="true" ht="171.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+    </row>
+    <row r="55" s="16" customFormat="true" ht="252.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="13" t="s">
         <v>129</v>
       </c>
       <c r="E55" s="3"/>
@@ -2314,32 +2298,32 @@
         <v>131</v>
       </c>
       <c r="H55" s="3"/>
-      <c r="I55" s="16"/>
-      <c r="J55" s="16"/>
-    </row>
-    <row r="56" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+    </row>
+    <row r="56" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-    </row>
-    <row r="57" s="17" customFormat="true" ht="303.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+    </row>
+    <row r="57" s="16" customFormat="true" ht="303.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D57" s="13" t="s">
         <v>134</v>
       </c>
       <c r="E57" s="3"/>
@@ -2352,117 +2336,117 @@
       <c r="H57" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="I57" s="16"/>
-      <c r="J57" s="16"/>
-    </row>
-    <row r="58" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+    </row>
+    <row r="58" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
-    </row>
-    <row r="59" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+    </row>
+    <row r="59" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="16"/>
-    </row>
-    <row r="60" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+    </row>
+    <row r="60" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="16"/>
-    </row>
-    <row r="61" s="10" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="s">
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+    </row>
+    <row r="61" s="9" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="E61" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="F61" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="10" t="s">
+      <c r="G61" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="62" s="10" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" s="19" customFormat="true" ht="388.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
+    <row r="62" s="9" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" s="18" customFormat="true" ht="388.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C63" s="18" t="s">
+      <c r="C63" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="18"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10" t="s">
+      <c r="D63" s="17"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="G63" s="10" t="s">
+      <c r="G63" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="H63" s="10" t="s">
+      <c r="H63" s="9" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="64" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-    </row>
-    <row r="65" s="17" customFormat="true" ht="316.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+    </row>
+    <row r="65" s="16" customFormat="true" ht="316.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D65" s="14" t="s">
+      <c r="D65" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="13" t="s">
         <v>152</v>
       </c>
       <c r="F65" s="3" t="s">
@@ -2474,67 +2458,67 @@
       <c r="H65" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I65" s="16"/>
-      <c r="J65" s="16"/>
-    </row>
-    <row r="66" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+    </row>
+    <row r="66" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="16"/>
-    </row>
-    <row r="67" s="22" customFormat="true" ht="216" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="20" t="s">
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+    </row>
+    <row r="67" s="18" customFormat="true" ht="216" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C67" s="21" t="s">
+      <c r="C67" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="D67" s="21"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20" t="s">
+      <c r="D67" s="17"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="G67" s="20" t="s">
+      <c r="G67" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="H67" s="20" t="s">
+      <c r="H67" s="9" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="68" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
-      <c r="H68" s="10"/>
-    </row>
-    <row r="69" s="17" customFormat="true" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="18" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="69" s="16" customFormat="true" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="D69" s="14" t="s">
+      <c r="D69" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="E69" s="14" t="s">
+      <c r="E69" s="13" t="s">
         <v>161</v>
       </c>
       <c r="F69" s="3" t="s">
@@ -2546,35 +2530,35 @@
       <c r="H69" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="I69" s="16"/>
-      <c r="J69" s="16"/>
-    </row>
-    <row r="70" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+    </row>
+    <row r="70" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="16"/>
-      <c r="J70" s="16"/>
-    </row>
-    <row r="71" s="17" customFormat="true" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+    </row>
+    <row r="71" s="16" customFormat="true" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C71" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="D71" s="14" t="s">
+      <c r="D71" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="E71" s="13" t="s">
         <v>168</v>
       </c>
       <c r="F71" s="3" t="s">
@@ -2584,35 +2568,35 @@
         <v>170</v>
       </c>
       <c r="H71" s="3"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="16"/>
-    </row>
-    <row r="72" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+    </row>
+    <row r="72" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
-      <c r="I72" s="16"/>
-      <c r="J72" s="16"/>
-    </row>
-    <row r="73" s="17" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+    </row>
+    <row r="73" s="16" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C73" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="D73" s="14" t="s">
+      <c r="D73" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="E73" s="14" t="s">
+      <c r="E73" s="13" t="s">
         <v>174</v>
       </c>
       <c r="F73" s="3" t="s">
@@ -2624,20 +2608,20 @@
       <c r="H73" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
-    </row>
-    <row r="74" s="17" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+    </row>
+    <row r="74" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
-      <c r="I74" s="16"/>
-      <c r="J74" s="16"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
     </row>
     <row r="75" customFormat="false" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7" t="s">
@@ -2646,22 +2630,22 @@
       <c r="B75" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C75" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D75" s="10" t="s">
+      <c r="D75" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E75" s="10"/>
-      <c r="F75" s="14" t="s">
+      <c r="E75" s="9"/>
+      <c r="F75" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="G75" s="10" t="s">
+      <c r="G75" s="9" t="s">
         <v>181</v>
       </c>
       <c r="H75" s="3"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3"/>
@@ -2672,8 +2656,8 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="16"/>
-      <c r="J76" s="16"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
     </row>
     <row r="77" customFormat="false" ht="374.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
@@ -2682,18 +2666,18 @@
       <c r="B77" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="C77" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D77" s="10" t="s">
+      <c r="D77" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E77" s="10"/>
+      <c r="E77" s="9"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="16"/>
-      <c r="J77" s="16"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3"/>
@@ -2704,60 +2688,60 @@
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="16"/>
-      <c r="J78" s="16"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
     </row>
     <row r="79" customFormat="false" ht="201.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B79" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C79" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10" t="s">
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="H79" s="10"/>
+      <c r="H79" s="9"/>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="7"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="10"/>
-      <c r="G80" s="10"/>
-      <c r="H80" s="10"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
     </row>
     <row r="81" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B81" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C81" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="D81" s="10" t="s">
+      <c r="D81" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="E81" s="10" t="s">
+      <c r="E81" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="F81" s="10" t="s">
+      <c r="F81" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="G81" s="10" t="s">
+      <c r="G81" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="H81" s="10" t="s">
+      <c r="H81" s="9" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2771,19 +2755,19 @@
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
-      <c r="I83" s="16"/>
-      <c r="J83" s="16"/>
-    </row>
-    <row r="84" s="23" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
+    </row>
+    <row r="84" s="19" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="85" s="4" customFormat="true" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
         <v>15</v>
@@ -2838,89 +2822,89 @@
       </c>
     </row>
     <row r="88" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" s="9" customFormat="true" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="9" t="s">
+    <row r="89" s="7" customFormat="true" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B89" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C89" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="D89" s="9" t="s">
+      <c r="D89" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="E89" s="9" t="s">
+      <c r="E89" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="F89" s="9" t="s">
+      <c r="F89" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G89" s="9" t="s">
+      <c r="G89" s="7" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
       <c r="E90" s="7"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
     </row>
     <row r="91" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B91" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="C91" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="D91" s="9" t="s">
         <v>216</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="F91" s="10" t="s">
+      <c r="F91" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="G91" s="10" t="s">
+      <c r="G91" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="H91" s="10" t="s">
+      <c r="H91" s="9" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="92" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" s="9" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="9" t="s">
+    <row r="93" s="7" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B93" s="9" t="s">
+      <c r="B93" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="C93" s="9" t="s">
+      <c r="C93" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="D93" s="9" t="s">
+      <c r="D93" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="E93" s="9" t="s">
+      <c r="E93" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="F93" s="9" t="s">
+      <c r="F93" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="G93" s="9" t="s">
+      <c r="G93" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="H93" s="9" t="s">
+      <c r="H93" s="7" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2948,7 +2932,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" s="12" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="97" s="4" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
         <v>15</v>

</xml_diff>